<commit_message>
feat: mos & buck selected
</commit_message>
<xml_diff>
--- a/sel/mosfet.xlsx
+++ b/sel/mosfet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guoyr\Desktop\foc-hw\sel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA064347-76C7-4A83-9CD6-9D3D879A9D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9C0746-549A-44BB-823C-E60D1AF7C607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14904" yWindow="1140" windowWidth="14796" windowHeight="12120" tabRatio="453" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="16656" tabRatio="344" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="126">
   <si>
     <t>https://github.com/odriverobotics/ODriveHardware</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -254,6 +254,295 @@
   </si>
   <si>
     <t>4@15A10V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://zhihui.lingjun.life/2020/07/02/foc/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>稚晖君foc驱动板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">irf7480mtrpbf </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>217@25℃
+137@100℃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>330@25℃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.95@10V
+1.6@6V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>123@132A10V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>31@132A10V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>44@132A10V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>21@30A10V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>70@30A10V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>68@30A10V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>58@30A10V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6680@25V1MHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1035@25V1MHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>700@25V1MHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>80@25℃
+60@100℃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>320@25℃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.82@10V
+3.47@7V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1029@25V1MHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>326@25V1MHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>21@25V1MHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17@80A32V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.8@80A32V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.8@80A32V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3@80A10V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2@80A10V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6@80A10V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/miaow-cn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iauc80n04s6n036</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jmsh0403bgq</t>
+  </si>
+  <si>
+    <t>未知foc驱动板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>145@25℃
+103@100℃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.2@10V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2086@20V1MHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1150@20V1MHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>60@20V1MHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>22@20A10V
+17.6@20A6V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9.2@20A10V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.3@20A10V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>63@10V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14.8@10V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>31@10V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>87@10V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iauc100n04s6n022</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100@25℃
+96@100℃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.77@10V
+2.11@7V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1862@25V1MHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>577@25V1MHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>29@25V1MHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>29@100A32V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8.3@100A32V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.2@100A32V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5@100A10V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3@100A10V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11@100A10V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6@100A10V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iauc60n06s5n074</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>60@25℃
+15@85℃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6@10V
+7.5@7V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1124@30V1MHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>284@30V1MHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14@30V1MHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.7@30A10V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.3@30A10V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.4@30A10V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3@30A10V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15.4@30A30V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5@30A30V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.9@30A30V</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -261,7 +550,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,13 +574,27 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -306,7 +609,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -320,14 +623,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -356,8 +665,8 @@
       <xdr:rowOff>93784</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="506614" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="文本框 1">
@@ -399,6 +708,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -433,7 +743,7 @@
                     <m:d>
                       <m:dPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="0">
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
@@ -458,7 +768,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="文本框 1">
@@ -534,8 +844,8 @@
       <xdr:rowOff>99646</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="435697" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="文本框 2">
@@ -577,6 +887,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -611,7 +922,7 @@
                     <m:d>
                       <m:dPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="0">
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
@@ -636,7 +947,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="文本框 2">
@@ -706,259 +1017,14 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>29308</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1017138" cy="181332"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="7" name="文本框 6">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C3A411D-0180-4127-8ABD-3640EB69EE17}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="6260123" y="0"/>
-              <a:ext cx="1017138" cy="181332"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:sSub>
-                      <m:sSubPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:sSubPr>
-                      <m:e>
-                        <m:f>
-                          <m:fPr>
-                            <m:type m:val="lin"/>
-                            <m:ctrlPr>
-                              <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="1">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                            </m:ctrlPr>
-                          </m:fPr>
-                          <m:num>
-                            <m:r>
-                              <m:rPr>
-                                <m:sty m:val="p"/>
-                              </m:rPr>
-                              <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                              <m:t>d</m:t>
-                            </m:r>
-                            <m:r>
-                              <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                              <m:t>𝑉</m:t>
-                            </m:r>
-                          </m:num>
-                          <m:den>
-                            <m:r>
-                              <m:rPr>
-                                <m:sty m:val="p"/>
-                              </m:rPr>
-                              <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                              <m:t>d</m:t>
-                            </m:r>
-                            <m:r>
-                              <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                              <m:t>𝑡</m:t>
-                            </m:r>
-                          </m:den>
-                        </m:f>
-                      </m:e>
-                      <m:sub>
-                        <m:r>
-                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝐷𝑆</m:t>
-                        </m:r>
-                      </m:sub>
-                    </m:sSub>
-                    <m:d>
-                      <m:dPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="0">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:dPr>
-                      <m:e>
-                        <m:f>
-                          <m:fPr>
-                            <m:type m:val="lin"/>
-                            <m:ctrlPr>
-                              <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="0">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                            </m:ctrlPr>
-                          </m:fPr>
-                          <m:num>
-                            <m:r>
-                              <m:rPr>
-                                <m:sty m:val="p"/>
-                              </m:rPr>
-                              <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                              <m:t>V</m:t>
-                            </m:r>
-                          </m:num>
-                          <m:den>
-                            <m:r>
-                              <m:rPr>
-                                <m:sty m:val="p"/>
-                              </m:rPr>
-                              <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                              <m:t>ns</m:t>
-                            </m:r>
-                          </m:den>
-                        </m:f>
-                      </m:e>
-                    </m:d>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100" i="0"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="7" name="文本框 6">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C3A411D-0180-4127-8ABD-3640EB69EE17}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="6260123" y="0"/>
-              <a:ext cx="1017138" cy="181332"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>〖</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>d𝑉∕d𝑡〗_𝐷𝑆 </a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>(</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>V∕ns)</a:t>
-              </a:r>
-              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100" i="0"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="364138" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="20" name="文本框 19">
@@ -1000,6 +1066,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1034,7 +1101,7 @@
                     <m:d>
                       <m:dPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="0">
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
@@ -1059,7 +1126,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="20" name="文本框 19">
@@ -1135,8 +1202,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="454740" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="21" name="文本框 20">
@@ -1178,6 +1245,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1212,7 +1280,7 @@
                     <m:d>
                       <m:dPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="0">
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
@@ -1237,7 +1305,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="21" name="文本框 20">
@@ -1313,8 +1381,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="585866" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="22" name="文本框 21">
@@ -1356,6 +1424,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1390,7 +1459,7 @@
                     <m:d>
                       <m:dPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="0">
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
@@ -1415,7 +1484,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="22" name="文本框 21">
@@ -1491,8 +1560,8 @@
       <xdr:rowOff>82061</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="802847" cy="185885"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="23" name="文本框 22">
@@ -1534,6 +1603,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1586,7 +1656,7 @@
                     <m:d>
                       <m:dPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="0">
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
@@ -1620,7 +1690,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="23" name="文本框 22">
@@ -1696,8 +1766,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="631583" cy="185885"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="24" name="文本框 23">
@@ -1739,6 +1809,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1791,7 +1862,7 @@
                     <m:d>
                       <m:dPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="0">
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
@@ -1816,7 +1887,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="24" name="文本框 23">
@@ -1892,8 +1963,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="620298" cy="185885"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="25" name="文本框 24">
@@ -1935,6 +2006,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1987,7 +2059,7 @@
                     <m:d>
                       <m:dPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="0">
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
@@ -2012,7 +2084,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="25" name="文本框 24">
@@ -2088,8 +2160,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="689356" cy="185885"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="26" name="文本框 25">
@@ -2131,6 +2203,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -2183,7 +2256,7 @@
                     <m:d>
                       <m:dPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="0">
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
@@ -2208,7 +2281,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="26" name="文本框 25">
@@ -2284,8 +2357,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="676339" cy="185885"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="27" name="文本框 26">
@@ -2327,6 +2400,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -2379,7 +2453,7 @@
                     <m:d>
                       <m:dPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="0">
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
@@ -2404,7 +2478,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="27" name="文本框 26">
@@ -2480,8 +2554,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="159146" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="28" name="文本框 27">
@@ -2523,6 +2597,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -2562,7 +2637,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="28" name="文本框 27">
@@ -2626,8 +2701,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="475643" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="29" name="文本框 28">
@@ -2669,6 +2744,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -2703,7 +2779,7 @@
                     <m:d>
                       <m:dPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="0">
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
@@ -2728,7 +2804,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="29" name="文本框 28">
@@ -2804,8 +2880,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="530082" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="30" name="文本框 29">
@@ -2847,6 +2923,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -2881,7 +2958,7 @@
                     <m:d>
                       <m:dPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="0">
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
@@ -2906,7 +2983,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="30" name="文本框 29">
@@ -2982,8 +3059,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="547394" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="31" name="文本框 30">
@@ -3025,6 +3102,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -3059,7 +3137,7 @@
                     <m:d>
                       <m:dPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="0">
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
@@ -3084,7 +3162,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="31" name="文本框 30">
@@ -3160,8 +3238,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="522772" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="32" name="文本框 31">
@@ -3203,6 +3281,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -3237,7 +3316,7 @@
                     <m:d>
                       <m:dPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="0">
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
@@ -3262,7 +3341,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="32" name="文本框 31">
@@ -3338,8 +3417,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="547329" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="33" name="文本框 32">
@@ -3381,6 +3460,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -3415,7 +3495,7 @@
                     <m:d>
                       <m:dPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="0">
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
@@ -3440,7 +3520,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="33" name="文本框 32">
@@ -3516,8 +3596,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="541174" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="34" name="文本框 33">
@@ -3559,6 +3639,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -3593,7 +3674,7 @@
                     <m:d>
                       <m:dPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="0">
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1100" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
@@ -3618,7 +3699,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="34" name="文本框 33">
@@ -3952,34 +4033,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T13"/>
+  <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.21875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.21875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" style="3" customWidth="1"/>
     <col min="4" max="4" width="7.21875" style="3" customWidth="1"/>
     <col min="5" max="5" width="12.5546875" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="3" customWidth="1"/>
     <col min="7" max="7" width="16.109375" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="15.88671875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="18.5546875" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.6640625" style="3" customWidth="1"/>
     <col min="11" max="11" width="14.5546875" style="3" customWidth="1"/>
     <col min="12" max="12" width="14.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.5546875" style="3" customWidth="1"/>
     <col min="14" max="14" width="13.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="18" width="14.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.6640625" style="3" customWidth="1"/>
-    <col min="20" max="16384" width="8.88671875" style="3"/>
+    <col min="19" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -4008,11 +4088,11 @@
       <c r="P1" s="7"/>
       <c r="Q1" s="7"/>
       <c r="R1" s="7"/>
-      <c r="T1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -4025,7 +4105,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:20" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -4047,7 +4127,7 @@
       <c r="G3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="I3" s="4" t="s">
@@ -4074,20 +4154,17 @@
       <c r="P3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="R3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="S3" s="3">
-        <v>6</v>
-      </c>
-      <c r="T3" s="5" t="s">
+      <c r="S3" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -4121,13 +4198,13 @@
       <c r="K4" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="6" t="s">
         <v>49</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="5" t="s">
         <v>51</v>
       </c>
       <c r="O4" s="4" t="s">
@@ -4136,33 +4213,30 @@
       <c r="P4" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="Q4" s="6" t="s">
+      <c r="Q4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="R4" s="6" t="s">
+      <c r="R4" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="S4" s="3">
-        <v>6.5</v>
-      </c>
-      <c r="T4" s="5" t="s">
+      <c r="S4" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="5">
         <v>68</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F5" s="4">
@@ -4204,26 +4278,312 @@
       <c r="R5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="T5" s="5" t="s">
+      <c r="S5" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="T13" s="3" t="s">
+    <row r="6" spans="1:21" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="3">
+        <v>40</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" s="3">
+        <v>868</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="3">
+        <v>40</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="R7" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="3">
+        <v>40</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8" s="3">
+        <v>581</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="8">
+        <v>40</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8">
+        <v>400</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="O9" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="P9" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q9" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="R9" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="S9" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+    </row>
+    <row r="10" spans="1:21" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" s="3">
+        <v>60</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="G10" s="3">
+        <v>60</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S13" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J19" s="3" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="O1:R1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="O1:R1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>